<commit_message>
issue in adding new excel sheet under src/main/resources
</commit_message>
<xml_diff>
--- a/7rMartSuperMarket/src/main/resources/testdata.xlsx
+++ b/7rMartSuperMarket/src/main/resources/testdata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="11016" windowHeight="2820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="loginpage" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="adduser" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -25,6 +26,21 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>usename</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>nee</t>
+  </si>
+  <si>
+    <t>neethu</t>
+  </si>
+  <si>
+    <t>nqww</t>
   </si>
 </sst>
 </file>
@@ -365,7 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -394,12 +410,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>112323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>112323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>54546465</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
new datas added to excel sheet
</commit_message>
<xml_diff>
--- a/7rMartSuperMarket/src/main/resources/testdata.xlsx
+++ b/7rMartSuperMarket/src/main/resources/testdata.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neethu\git\7rMartSuperMarketnew\7rMartSuperMarket\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB557A28-784A-41F3-A715-187500996698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="11016" windowHeight="2820" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginpage" sheetId="1" r:id="rId1"/>
     <sheet name="adduser" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:K8"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -41,12 +46,18 @@
   </si>
   <si>
     <t>nqww</t>
+  </si>
+  <si>
+    <t>ertrty</t>
+  </si>
+  <si>
+    <t>keva</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,14 +99,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -133,7 +147,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -205,7 +219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -378,7 +392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -409,14 +423,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -450,13 +467,29 @@
         <v>54546465</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>23435355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>132154667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>